<commit_message>
Added GetAppCredentials process and corresponding dependencies.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>URL for ACME System 1</t>
   </si>
   <si>
-    <t>AcmeURL</t>
-  </si>
-  <si>
     <t>MyQueue</t>
   </si>
   <si>
@@ -134,13 +131,16 @@
     <t>AcmeFramework</t>
   </si>
   <si>
-    <t>AcmeCredential</t>
-  </si>
-  <si>
     <t>AcmeCredentials</t>
   </si>
   <si>
     <t>Credentials for ACME System 1</t>
+  </si>
+  <si>
+    <t>System1Credential</t>
+  </si>
+  <si>
+    <t>System1URL</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -570,15 +570,15 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -592,7 +592,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -600,24 +600,24 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1622,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Competed implementation of InitAllApplications and CloseAllApplications.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -143,13 +143,49 @@
     <t>System1URL</t>
   </si>
   <si>
-    <t>ExceptionsEmail</t>
-  </si>
-  <si>
     <t>exceptions@acme-test.com</t>
   </si>
   <si>
-    <t>Email for notifications due to errors in ACME System1 automations</t>
+    <t>EmailCredentials</t>
+  </si>
+  <si>
+    <t>Credentials for email account to send out notifications.</t>
+  </si>
+  <si>
+    <t>ExceptionsDestinationEmail</t>
+  </si>
+  <si>
+    <t>SourceEmailCredentials</t>
+  </si>
+  <si>
+    <t>Email to send notifications to in case of errors in automations</t>
+  </si>
+  <si>
+    <t>Header of the email notification</t>
+  </si>
+  <si>
+    <t>ExceptionsEmailBody</t>
+  </si>
+  <si>
+    <t>Body of email notification.</t>
+  </si>
+  <si>
+    <t>ExceptionsEmailSubject</t>
+  </si>
+  <si>
+    <t>ExceptionsEmailSender</t>
+  </si>
+  <si>
+    <t>Sender name to be shown in email notification</t>
+  </si>
+  <si>
+    <t>Hello! Something happened. Please check logs.</t>
+  </si>
+  <si>
+    <t>Error occurred.</t>
+  </si>
+  <si>
+    <t>Security Cash Automation</t>
   </si>
 </sst>
 </file>
@@ -211,7 +247,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -223,6 +259,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -530,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,7 +578,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -641,22 +678,62 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>43</v>
+      <c r="C9" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1645,7 +1722,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Fixes to GetTransactionData due to missing first record.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -701,39 +701,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1733,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1859,9 +1829,39 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fixes to sending email functionality
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -143,12 +143,6 @@
     <t>System1URL</t>
   </si>
   <si>
-    <t>exceptions@acme-test.com</t>
-  </si>
-  <si>
-    <t>EmailCredentials</t>
-  </si>
-  <si>
     <t>Credentials for email account to send out notifications.</t>
   </si>
   <si>
@@ -158,18 +152,9 @@
     <t>SourceEmailCredentials</t>
   </si>
   <si>
-    <t>Email to send notifications to in case of errors in automations</t>
-  </si>
-  <si>
     <t>Header of the email notification</t>
   </si>
   <si>
-    <t>ExceptionsEmailBody</t>
-  </si>
-  <si>
-    <t>Body of email notification.</t>
-  </si>
-  <si>
     <t>ExceptionsEmailSubject</t>
   </si>
   <si>
@@ -179,13 +164,19 @@
     <t>Sender name to be shown in email notification</t>
   </si>
   <si>
-    <t>Hello! Something happened. Please check logs.</t>
-  </si>
-  <si>
-    <t>Error occurred.</t>
-  </si>
-  <si>
-    <t>Security Cash Automation</t>
+    <t>Client Security Hash Robot</t>
+  </si>
+  <si>
+    <t>Error in CalculateSecurityHash robot.</t>
+  </si>
+  <si>
+    <t>GmailCredentials</t>
+  </si>
+  <si>
+    <t>AcmeExceptionsEmail</t>
+  </si>
+  <si>
+    <t>Destination email for exceptions notifications (exceptions@acme-test.com)</t>
   </si>
 </sst>
 </file>
@@ -247,7 +238,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -260,6 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -575,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -681,28 +673,41 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="5" t="s">
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1688,11 +1693,10 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId1" display="vovcheg.1984@mail.ru"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1703,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1829,39 +1833,9 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2845,8 +2819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2893,7 +2867,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Corrections to update WI flow.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1707,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2819,7 +2819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>